<commit_message>
docs: Completar revision tecnica formal y correccion del modelo de casos de uso.
</commit_message>
<xml_diff>
--- a/2. Etapa de elaboración/Iteración 2/Plan de pruebas/Matriz RQS-CU.xlsx
+++ b/2. Etapa de elaboración/Iteración 2/Plan de pruebas/Matriz RQS-CU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Desktop\UNI\Analista de sistemas\Tercer año\Segundo cuatrimestre\Laboratorio de desarrollo de software\Git\develop\2. Etapa de elaboración\Iteración 2\Plan de pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D635EEF-440F-40D4-AC13-897E5F6D0CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1402F812-0917-45B4-BD8E-7817C367E2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>CU1: AUTENTIFICARSE</t>
   </si>
@@ -64,66 +64,12 @@
     <t>CU12: REALIZAR ANALISIS DE RIESGOS</t>
   </si>
   <si>
-    <t>RQS1: REGISTRAR USUARIO</t>
-  </si>
-  <si>
-    <t>RQS2: ASIGNAR PERFIL</t>
-  </si>
-  <si>
     <t>RQS3: INICIAR SESION</t>
   </si>
   <si>
-    <t>RQS4: CREAR PROYECTO</t>
-  </si>
-  <si>
     <t>RQS5: ASIGNAR PARTICIPANTES</t>
   </si>
   <si>
-    <t>RQS6: MODIFICAR INFORMACION DE PROYECTO</t>
-  </si>
-  <si>
-    <t>RQS7: AÑADIR RIESGO</t>
-  </si>
-  <si>
-    <t>RQS8: MODIFICAR RIESGO</t>
-  </si>
-  <si>
-    <t>RQS9: AÑADIR, MODIFICAR Y ELIMINAR CATEGORIA</t>
-  </si>
-  <si>
-    <t>RQS10: EVALUAR RIESGO</t>
-  </si>
-  <si>
-    <t>RQS11: MOSTRAR RIESGOS PRIORITARIOS</t>
-  </si>
-  <si>
-    <t>RQS12: GENERAR PLANES</t>
-  </si>
-  <si>
-    <t>RQS13: MARCAR EVALUACIONES PENDIENTES</t>
-  </si>
-  <si>
-    <t>RQS14: MARCAR PLANIFICACIONES PENDIENTES</t>
-  </si>
-  <si>
-    <t>RQS15: GENERAR INFORMES</t>
-  </si>
-  <si>
-    <t>RQS16: GENERAR RESUMENES Y GRAFICOS</t>
-  </si>
-  <si>
-    <t>RQS17: PRESENTAR EVOLUCION DE RIESGOS</t>
-  </si>
-  <si>
-    <t>RQS18: EXPORTAR ARCHIVOS</t>
-  </si>
-  <si>
-    <t>RQS19: GESTIONAR ITERACIONES</t>
-  </si>
-  <si>
-    <t>RQS20: SOLICITAR INFORMES</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -133,7 +79,55 @@
     <t>RESULTADO:</t>
   </si>
   <si>
-    <t>RQS21: MODIFICAR PLAN</t>
+    <t>RQS1: ADMINISTRAR USUARIO</t>
+  </si>
+  <si>
+    <t>RQS2: ADMINISTRAR PERFILES DE USUARIO</t>
+  </si>
+  <si>
+    <t>RQS4: GESTIONAR PROYECTO</t>
+  </si>
+  <si>
+    <t>RQS6: AÑADIR RIESGO</t>
+  </si>
+  <si>
+    <t>RQS7: MODIFICAR Y ELIMINAR RIESGO</t>
+  </si>
+  <si>
+    <t>RQS9: EVALUAR RIESGO</t>
+  </si>
+  <si>
+    <t>RQS10: MOSTRAR RIESGOS PRIORITARIOS</t>
+  </si>
+  <si>
+    <t>RQS11: GENERAR PLANES</t>
+  </si>
+  <si>
+    <t>RQS12: MARCAR ACCIONES PENDIENTES</t>
+  </si>
+  <si>
+    <t>RQS13: GENERAR INFORMES</t>
+  </si>
+  <si>
+    <t>RQS14: PRESENTAR RESUMENES Y GRAFICOS</t>
+  </si>
+  <si>
+    <t>RQS15: EXPORTAR ARCHIVOS</t>
+  </si>
+  <si>
+    <t>RQS16: GESTIONAR ITERACIONES</t>
+  </si>
+  <si>
+    <t>RQS17: SOLICITAR INFORMES</t>
+  </si>
+  <si>
+    <t>RQS18: MODIFICAR PLAN</t>
+  </si>
+  <si>
+    <t>RQS8: Gestionar categorias</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -465,13 +459,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -480,33 +474,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,16 +829,16 @@
         <v>11</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -861,13 +855,13 @@
         <v>SI</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -880,16 +874,16 @@
       <c r="L3" s="2"/>
       <c r="M3" s="3"/>
       <c r="N3" s="9" t="str">
-        <f t="shared" ref="N3:N20" si="0">IF(COUNTIF(B3:M3,"X")&lt;1, "NO", "SI")</f>
+        <f t="shared" ref="N3:N17" si="0">IF(COUNTIF(B3:M3,"X")&lt;1, "NO", "SI")</f>
         <v>SI</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -907,14 +901,14 @@
         <v>SI</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -932,12 +926,12 @@
     </row>
     <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -953,16 +947,16 @@
         <v>SI</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -976,17 +970,17 @@
         <v>SI</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -999,18 +993,18 @@
         <v>SI</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1022,19 +1016,19 @@
         <v>SI</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -1045,9 +1039,9 @@
         <v>SI</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1056,21 +1050,23 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="3"/>
+      <c r="M11" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="N11" s="9" t="str">
         <f t="shared" si="0"/>
         <v>SI</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1078,24 +1074,22 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="M12" s="3"/>
       <c r="N12" s="9" t="str">
         <f t="shared" si="0"/>
         <v>SI</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1103,22 +1097,26 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I13" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="3"/>
+      <c r="M13" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="N13" s="9" t="str">
         <f t="shared" si="0"/>
         <v>SI</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1126,24 +1124,22 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="K14" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="L14" s="2"/>
-      <c r="M14" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="M14" s="3"/>
       <c r="N14" s="9" t="str">
         <f t="shared" si="0"/>
         <v>SI</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1152,15 +1148,13 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="K15" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="L15" s="2"/>
-      <c r="M15" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="M15" s="3"/>
       <c r="N15" s="9" t="str">
         <f t="shared" si="0"/>
         <v>SI</v>
@@ -1168,7 +1162,7 @@
     </row>
     <row r="16" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1179,34 +1173,32 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="M16" s="3"/>
       <c r="N16" s="9" t="str">
         <f t="shared" si="0"/>
         <v>SI</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="3"/>
       <c r="N17" s="9" t="str">
@@ -1214,208 +1206,137 @@
         <v>SI</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>SI</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M19" s="3"/>
-      <c r="N19" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>SI</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="18" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>SI</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="10" t="str">
+        <f>IF(COUNTIF(B18:M18,"X")&lt;1, "NO", "SI")</f>
+        <v>SI</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L21" s="4"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="10" t="str">
-        <f>IF(COUNTIF(B21:M21,"X")&lt;1, "NO", "SI")</f>
-        <v>SI</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="19"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="10" t="str">
+        <f>IF(COUNTIF(B19:M19,"X")&lt;1, "NO", "SI")</f>
+        <v>SI</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="7" t="str">
+        <f>IF(COUNTIF(B2:B18,"X")&lt;1, "NO", "SI")</f>
+        <v>SI</v>
+      </c>
+      <c r="C20" s="7" t="str">
+        <f t="shared" ref="C20:M20" si="1">IF(COUNTIF(C2:C18,"X")&lt;1, "NO", "SI")</f>
+        <v>SI</v>
+      </c>
+      <c r="D20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>SI</v>
+      </c>
+      <c r="E20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>SI</v>
+      </c>
+      <c r="F20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>SI</v>
+      </c>
+      <c r="G20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>SI</v>
+      </c>
+      <c r="H20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>SI</v>
+      </c>
+      <c r="I20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>SI</v>
+      </c>
+      <c r="J20" s="7" t="str">
+        <f>IF(COUNTIF(J2:J19,"X")&lt;1, "NO", "SI")</f>
+        <v>SI</v>
+      </c>
+      <c r="K20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>SI</v>
+      </c>
+      <c r="L20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>SI</v>
+      </c>
+      <c r="M20" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>SI</v>
+      </c>
+      <c r="N20" s="12">
+        <f>COUNTIF(A20:M20,"NO")+COUNTIF(N2:N19,"NO")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:14" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="18" t="str">
+        <f>CONCATENATE(COUNTIF(A20:M20,"NO"), " CASOS DE USO INNECESARIOS")</f>
+        <v>0 CASOS DE USO INNECESARIOS</v>
+      </c>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="10" t="str">
-        <f>IF(COUNTIF(B22:M22,"X")&lt;1, "NO", "SI")</f>
-        <v>SI</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="7" t="str">
-        <f>IF(COUNTIF(B2:B21,"X")&lt;1, "NO", "SI")</f>
-        <v>SI</v>
-      </c>
-      <c r="C23" s="7" t="str">
-        <f t="shared" ref="C23:M23" si="1">IF(COUNTIF(C2:C21,"X")&lt;1, "NO", "SI")</f>
-        <v>SI</v>
-      </c>
-      <c r="D23" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>SI</v>
-      </c>
-      <c r="E23" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>SI</v>
-      </c>
-      <c r="F23" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>SI</v>
-      </c>
-      <c r="G23" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>SI</v>
-      </c>
-      <c r="H23" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>SI</v>
-      </c>
-      <c r="I23" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>SI</v>
-      </c>
-      <c r="J23" s="7" t="str">
-        <f>IF(COUNTIF(J2:J22,"X")&lt;1, "NO", "SI")</f>
-        <v>SI</v>
-      </c>
-      <c r="K23" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>SI</v>
-      </c>
-      <c r="L23" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>SI</v>
-      </c>
-      <c r="M23" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>SI</v>
-      </c>
-      <c r="N23" s="14">
-        <f>COUNTIF(A23:M23,"NO")+COUNTIF(N2:N22,"NO")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:14" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="16" t="str">
-        <f>CONCATENATE(COUNTIF(A23:M23,"NO"), " CASOS DE USO INNECESARIOS")</f>
-        <v>0 CASOS DE USO INNECESARIOS</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="16" t="str">
-        <f>CONCATENATE(COUNTIF(N2:N22,"NO"), " REQUERIMIENTOS NO SATISFECHOS")</f>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18" t="str">
+        <f>CONCATENATE(COUNTIF(N2:N19,"NO"), " REQUERIMIENTOS NO SATISFECHOS")</f>
         <v>0 REQUERIMIENTOS NO SATISFECHOS</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="17"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>